<commit_message>
Adding company cidr to template
</commit_message>
<xml_diff>
--- a/Input_Enterprise_networks.xlsx
+++ b/Input_Enterprise_networks.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580CBB63-7BAF-4483-8D38-DA28CD54386B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5895E20D-C574-4DC7-99D7-8D8B5C956AF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30870" yWindow="3300" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Company_cidr" sheetId="13" r:id="rId1"/>
@@ -312,7 +312,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="166">
   <si>
     <t>Please do not delete any of these rows!</t>
   </si>
@@ -723,6 +723,93 @@
   </si>
   <si>
     <t>Insight_tempe_lab</t>
+  </si>
+  <si>
+    <t>172.28.40.16/29</t>
+  </si>
+  <si>
+    <t>172.28.40.24/29</t>
+  </si>
+  <si>
+    <t>EN_Wireless_Users_44</t>
+  </si>
+  <si>
+    <t>172.28.44.0/24</t>
+  </si>
+  <si>
+    <t>10.248.0.0/16</t>
+  </si>
+  <si>
+    <t>SDA_POV</t>
+  </si>
+  <si>
+    <t>10.123.0.0/16</t>
+  </si>
+  <si>
+    <t>10.124.0.0/16</t>
+  </si>
+  <si>
+    <t>10.125.0.0/16</t>
+  </si>
+  <si>
+    <t>10.126.0.0/16</t>
+  </si>
+  <si>
+    <t>10.127.0.0/16</t>
+  </si>
+  <si>
+    <t>Wireless_net1</t>
+  </si>
+  <si>
+    <t>DNAC_mgmt</t>
+  </si>
+  <si>
+    <t>Wireless_net3</t>
+  </si>
+  <si>
+    <t>SilverPeak_mgmt</t>
+  </si>
+  <si>
+    <t>172.17.25.0/24</t>
+  </si>
+  <si>
+    <t>EMEA_servers</t>
+  </si>
+  <si>
+    <t>172.18.153.0/24</t>
+  </si>
+  <si>
+    <t>Singapore_servers</t>
+  </si>
+  <si>
+    <t>172.19.120.0/24</t>
+  </si>
+  <si>
+    <t>172.23.107.0/24</t>
+  </si>
+  <si>
+    <t>APAC_servers</t>
+  </si>
+  <si>
+    <t>172.24.32.96/29</t>
+  </si>
+  <si>
+    <t>ATL_servers</t>
+  </si>
+  <si>
+    <t>APIC-EM_System</t>
+  </si>
+  <si>
+    <t>172.30.254.0/24</t>
+  </si>
+  <si>
+    <t>172.31.150.0/23</t>
+  </si>
+  <si>
+    <t>172.28.40.0/29</t>
+  </si>
+  <si>
+    <t>172.28.40.8/29</t>
   </si>
 </sst>
 </file>
@@ -1133,13 +1220,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -1547,10 +1632,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1609,253 +1694,406 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>164</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>165</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>137</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>138</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>140</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>141</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>143</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>144</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>145</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>146</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>147</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="B30" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>104</v>
+        <v>42</v>
       </c>
       <c r="B32" t="s">
-        <v>105</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>106</v>
+        <v>44</v>
       </c>
       <c r="B33" t="s">
-        <v>107</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>109</v>
+        <v>46</v>
       </c>
       <c r="B34" t="s">
-        <v>108</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>110</v>
+        <v>48</v>
       </c>
       <c r="B35" t="s">
-        <v>111</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>112</v>
+        <v>50</v>
       </c>
       <c r="B36" t="s">
-        <v>113</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>58</v>
+      </c>
+      <c r="B40" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>62</v>
+      </c>
+      <c r="B42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>104</v>
+      </c>
+      <c r="B43" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>106</v>
+      </c>
+      <c r="B44" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>109</v>
+      </c>
+      <c r="B45" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>110</v>
+      </c>
+      <c r="B46" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>112</v>
+      </c>
+      <c r="B47" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>122</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B48" t="s">
         <v>123</v>
       </c>
     </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>152</v>
+      </c>
+      <c r="B49" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>154</v>
+      </c>
+      <c r="B50" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>156</v>
+      </c>
+      <c r="B51" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>157</v>
+      </c>
+      <c r="B52" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>157</v>
+      </c>
+      <c r="B53" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>159</v>
+      </c>
+      <c r="B54" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>162</v>
+      </c>
+      <c r="B55" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>163</v>
+      </c>
+      <c r="B56" t="s">
+        <v>153</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>